<commit_message>
Update latest features and security configs
</commit_message>
<xml_diff>
--- a/Template_egfulfill_SKU_unrestricted_all_B.xlsx
+++ b/Template_egfulfill_SKU_unrestricted_all_B.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Code Kiem Tien\Rip egfulfill Jack NG\egfulfill-clone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D5EE83C-CB43-49B7-AB5E-9C515980A84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDD9F75-E063-427A-8D89-75BBA2A675DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6495" yWindow="3360" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="49">
   <si>
     <t>ORDER ID</t>
   </si>
@@ -106,9 +106,6 @@
     <t>TYPE 4</t>
   </si>
   <si>
-    <t>ORDER20213</t>
-  </si>
-  <si>
     <t>BLACK</t>
   </si>
   <si>
@@ -136,14 +133,50 @@
     <t>HOODIE-PREM</t>
   </si>
   <si>
-    <t>ORDER2026</t>
+    <t>TSHIRT-BASIC</t>
+  </si>
+  <si>
+    <t>WHITE</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>557 wtf street, California, USA, 7393</t>
+  </si>
+  <si>
+    <t>wataonima</t>
+  </si>
+  <si>
+    <t>cho anh xin 2 vi</t>
+  </si>
+  <si>
+    <t>CENTER_CHEST</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/u/0/my-drive</t>
+  </si>
+  <si>
+    <t>LEFT_CHEST</t>
+  </si>
+  <si>
+    <t>name: john</t>
+  </si>
+  <si>
+    <t>ORDER20211</t>
+  </si>
+  <si>
+    <t>ORDER2030</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -173,6 +206,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -219,7 +259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -242,11 +282,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -283,11 +335,19 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="16">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -361,6 +421,142 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF3F3F3"/>
@@ -387,9 +583,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Template-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="11"/>
-      <tableStyleElement type="firstRowStripe" dxfId="10"/>
-      <tableStyleElement type="secondRowStripe" dxfId="9"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="secondRowStripe" dxfId="13"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -404,10 +600,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:B3" headerRowCount="0">
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:F3" headerRowCount="0">
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{F607C538-851D-42EE-AE9E-CDA307FD6183}" name="Column3" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{994051C2-E25E-4E88-B206-58ECA77C1B08}" name="Column4" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{D19FDE43-FA07-47B7-B497-BC8A37832D24}" name="Column5" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{B7DDEB87-0577-4BEF-BE8B-A0BAC4B56A8F}" name="Column6" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Template-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -617,7 +817,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -648,7 +848,7 @@
     <col min="27" max="27" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,43 +933,43 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="10">
         <v>2</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="10"/>
       <c r="K2" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="M2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>34</v>
-      </c>
       <c r="N2" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P2" s="10"/>
       <c r="Q2" s="12"/>
@@ -784,26 +984,54 @@
       <c r="Z2" s="12"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="10">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>39</v>
+      </c>
       <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="H3" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
+      <c r="K3" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>46</v>
+      </c>
       <c r="R3" s="10"/>
       <c r="S3" s="10"/>
       <c r="T3" s="10"/>
@@ -815,7 +1043,7 @@
       <c r="Z3" s="10"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -844,7 +1072,7 @@
       <c r="Z4" s="10"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -873,7 +1101,7 @@
       <c r="Z5" s="10"/>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -902,7 +1130,7 @@
       <c r="Z6" s="10"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -931,7 +1159,7 @@
       <c r="Z7" s="10"/>
       <c r="AA7" s="10"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -960,7 +1188,7 @@
       <c r="Z8" s="10"/>
       <c r="AA8" s="10"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -989,7 +1217,7 @@
       <c r="Z9" s="10"/>
       <c r="AA9" s="10"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -1018,7 +1246,7 @@
       <c r="Z10" s="10"/>
       <c r="AA10" s="10"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -1047,7 +1275,7 @@
       <c r="Z11" s="10"/>
       <c r="AA11" s="10"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -1076,7 +1304,7 @@
       <c r="Z12" s="10"/>
       <c r="AA12" s="10"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -1105,7 +1333,7 @@
       <c r="Z13" s="10"/>
       <c r="AA13" s="10"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -1134,7 +1362,7 @@
       <c r="Z14" s="10"/>
       <c r="AA14" s="10"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -1163,7 +1391,7 @@
       <c r="Z15" s="10"/>
       <c r="AA15" s="10"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -1192,7 +1420,7 @@
       <c r="Z16" s="10"/>
       <c r="AA16" s="10"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -1221,7 +1449,7 @@
       <c r="Z17" s="10"/>
       <c r="AA17" s="10"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -1250,7 +1478,7 @@
       <c r="Z18" s="10"/>
       <c r="AA18" s="10"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -1279,7 +1507,7 @@
       <c r="Z19" s="10"/>
       <c r="AA19" s="10"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -1308,7 +1536,7 @@
       <c r="Z20" s="10"/>
       <c r="AA20" s="10"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -1337,7 +1565,7 @@
       <c r="Z21" s="10"/>
       <c r="AA21" s="10"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
       <c r="C22" s="10"/>
@@ -1366,7 +1594,7 @@
       <c r="Z22" s="10"/>
       <c r="AA22" s="10"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -1395,7 +1623,7 @@
       <c r="Z23" s="10"/>
       <c r="AA23" s="10"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -1424,7 +1652,7 @@
       <c r="Z24" s="10"/>
       <c r="AA24" s="10"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
@@ -1453,7 +1681,7 @@
       <c r="Z25" s="10"/>
       <c r="AA25" s="10"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
@@ -1482,7 +1710,7 @@
       <c r="Z26" s="10"/>
       <c r="AA26" s="10"/>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
@@ -1511,7 +1739,7 @@
       <c r="Z27" s="10"/>
       <c r="AA27" s="10"/>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -1540,7 +1768,7 @@
       <c r="Z28" s="10"/>
       <c r="AA28" s="10"/>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="10"/>
       <c r="C29" s="10"/>
@@ -1569,7 +1797,7 @@
       <c r="Z29" s="10"/>
       <c r="AA29" s="10"/>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="10"/>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -1598,7 +1826,7 @@
       <c r="Z30" s="10"/>
       <c r="AA30" s="10"/>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
       <c r="B31" s="10"/>
       <c r="C31" s="10"/>
@@ -1627,7 +1855,7 @@
       <c r="Z31" s="10"/>
       <c r="AA31" s="10"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -1656,7 +1884,7 @@
       <c r="Z32" s="10"/>
       <c r="AA32" s="10"/>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -1685,7 +1913,7 @@
       <c r="Z33" s="10"/>
       <c r="AA33" s="10"/>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -1714,7 +1942,7 @@
       <c r="Z34" s="10"/>
       <c r="AA34" s="10"/>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -1743,7 +1971,7 @@
       <c r="Z35" s="10"/>
       <c r="AA35" s="10"/>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -29805,10 +30033,12 @@
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="N2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M3" r:id="rId3" xr:uid="{1A8D7337-2047-4A85-BC55-F67F8C5B1A9E}"/>
+    <hyperlink ref="N3" r:id="rId4" xr:uid="{9BBB6211-8512-47CE-93DF-7563B015DE7A}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>